<commit_message>
Avance en la clase Definitions - Reprogramación mismo pagaré
</commit_message>
<xml_diff>
--- a/target/DatosExcel/DatosCreditoEmpresarialReprogramacionOtroPagare.xlsx
+++ b/target/DatosExcel/DatosCreditoEmpresarialReprogramacionOtroPagare.xlsx
@@ -92,9 +92,6 @@
     <t>6</t>
   </si>
   <si>
-    <t>22114387</t>
-  </si>
-  <si>
     <t>Modalidad Amortización</t>
   </si>
   <si>
@@ -104,9 +101,6 @@
     <t>Número Cuotas</t>
   </si>
   <si>
-    <t>080-01-0840793</t>
-  </si>
-  <si>
     <t>13/12/2021</t>
   </si>
   <si>
@@ -150,6 +144,12 @@
   </si>
   <si>
     <t>Prueba</t>
+  </si>
+  <si>
+    <t>15979240</t>
+  </si>
+  <si>
+    <t>080-01-6913172</t>
   </si>
 </sst>
 </file>
@@ -512,7 +512,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
@@ -548,7 +550,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -557,7 +559,7 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>13</v>
@@ -566,34 +568,34 @@
         <v>14</v>
       </c>
       <c r="I1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="K1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>40</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>17</v>
@@ -610,7 +612,7 @@
     </row>
     <row r="2" spans="1:22" s="7" customFormat="1">
       <c r="A2" s="4" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>6</v>
@@ -619,22 +621,22 @@
         <v>10</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>7</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>15</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="J2" s="5" t="s">
         <v>4</v>
@@ -652,16 +654,16 @@
         <v>21</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="P2" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="R2" s="6" t="s">
         <v>39</v>
-      </c>
-      <c r="Q2" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="R2" s="6" t="s">
-        <v>41</v>
       </c>
       <c r="S2" s="6" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
Avance de la clase Definitions para Reprogramación otro pagaré
</commit_message>
<xml_diff>
--- a/target/DatosExcel/DatosCreditoEmpresarialReprogramacionOtroPagare.xlsx
+++ b/target/DatosExcel/DatosCreditoEmpresarialReprogramacionOtroPagare.xlsx
@@ -50,9 +50,6 @@
     <t>OFICIO MULTIPLE N° 5345</t>
   </si>
   <si>
-    <t>Cronograma de Pagos</t>
-  </si>
-  <si>
     <t>Modalidad Pago</t>
   </si>
   <si>
@@ -101,9 +98,6 @@
     <t>Número Cuotas</t>
   </si>
   <si>
-    <t>13/12/2021</t>
-  </si>
-  <si>
     <t>REPROGRAMACION EN OTRO PAGARE</t>
   </si>
   <si>
@@ -150,6 +144,12 @@
   </si>
   <si>
     <t>080-01-6913172</t>
+  </si>
+  <si>
+    <t>20/12/2021</t>
+  </si>
+  <si>
+    <t>Cronograma Pagos</t>
   </si>
 </sst>
 </file>
@@ -512,9 +512,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
@@ -550,7 +548,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -559,117 +557,117 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="O1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="Q1" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>38</v>
-      </c>
       <c r="S1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="U1" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="V1" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:22" s="7" customFormat="1">
       <c r="A2" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>7</v>
       </c>
       <c r="F2" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I2" s="4" t="s">
         <v>28</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>30</v>
       </c>
       <c r="J2" s="5" t="s">
         <v>4</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="L2" s="5" t="s">
         <v>5</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="P2" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="R2" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="Q2" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="R2" s="6" t="s">
-        <v>39</v>
-      </c>
       <c r="S2" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="T2" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="U2"/>
       <c r="V2"/>

</xml_diff>

<commit_message>
Avance de la clase Definitions hasta el paso de Grabar para Reprogramación Otro Pagaré
</commit_message>
<xml_diff>
--- a/target/DatosExcel/DatosCreditoEmpresarialReprogramacionOtroPagare.xlsx
+++ b/target/DatosExcel/DatosCreditoEmpresarialReprogramacionOtroPagare.xlsx
@@ -128,9 +128,6 @@
     <t>Fecha Desembolso</t>
   </si>
   <si>
-    <t>Forma Ddesembolso</t>
-  </si>
-  <si>
     <t>EFECTIVO</t>
   </si>
   <si>
@@ -150,6 +147,9 @@
   </si>
   <si>
     <t>Cronograma Pagos</t>
+  </si>
+  <si>
+    <t>Forma Desembolso</t>
   </si>
 </sst>
 </file>
@@ -536,7 +536,7 @@
     <col min="18" max="18" width="17.7109375" customWidth="1"/>
     <col min="19" max="19" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="20" max="20" width="10.140625" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="17" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="21.140625" customWidth="1" collapsed="1"/>
     <col min="22" max="22" width="53.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
@@ -587,13 +587,13 @@
         <v>31</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="Q1" s="2" t="s">
         <v>33</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>16</v>
@@ -610,7 +610,7 @@
     </row>
     <row r="2" spans="1:22" s="7" customFormat="1">
       <c r="A2" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>6</v>
@@ -631,7 +631,7 @@
         <v>14</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>28</v>
@@ -640,7 +640,7 @@
         <v>4</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L2" s="5" t="s">
         <v>5</v>
@@ -655,13 +655,13 @@
         <v>32</v>
       </c>
       <c r="P2" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q2" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="R2" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="S2" s="6" t="s">
         <v>19</v>

</xml_diff>